<commit_message>
added inoise_mover and inoise_fire and juggle with phase
</commit_message>
<xml_diff>
--- a/readkeyboard_options.xlsx
+++ b/readkeyboard_options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeffKarle\Documents\cinder_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33361A43-79A8-4CC0-A483-8F8BA66E7814}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A80FBB-EE7B-4BCF-BFF2-8858C2D0AEF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27615" yWindow="3870" windowWidth="18375" windowHeight="15885" xr2:uid="{91536ED5-E4E4-4F8E-9A8A-8957252223C5}"/>
+    <workbookView xWindow="-27615" yWindow="3870" windowWidth="18375" windowHeight="15885" activeTab="1" xr2:uid="{91536ED5-E4E4-4F8E-9A8A-8957252223C5}"/>
   </bookViews>
   <sheets>
     <sheet name="keyboard" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="208">
   <si>
     <t>letter</t>
   </si>
@@ -665,6 +665,15 @@
   </si>
   <si>
     <t>juggle_pal_individual_ring_onedir_phase</t>
+  </si>
+  <si>
+    <t>inoise_mover</t>
+  </si>
+  <si>
+    <t>inoise_fire</t>
+  </si>
+  <si>
+    <t>jug16_phase</t>
   </si>
 </sst>
 </file>
@@ -868,7 +877,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="53">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1047,26 +1068,26 @@
   <autoFilter ref="C4:I18" xr:uid="{BB459464-8D55-4078-AEB0-B3756A24CE71}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6BA9E6BE-A65A-44B5-93BA-A9004172E176}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{3F544982-2614-4EBC-B5CD-9E2EEB5E2F9E}" name="this_rot" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{9816F04B-5C36-4613-8079-6EF4AF805F6B}" name="this_delay" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{0E24C419-693F-4DC7-A454-02E431D95E72}" name="target_palette" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{3FB5B42A-1E5E-46F4-98F5-AAEC25ECACBE}" name="bg_clr" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{767B200D-BA70-439B-94A5-74CB8576CAA0}" name="bg_bri" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{3986F5DC-2BA5-44B0-A8F4-7A7ACEA7BCB1}" name="this_fade" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{3F544982-2614-4EBC-B5CD-9E2EEB5E2F9E}" name="this_rot" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{9816F04B-5C36-4613-8079-6EF4AF805F6B}" name="this_delay" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{0E24C419-693F-4DC7-A454-02E431D95E72}" name="target_palette" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{3FB5B42A-1E5E-46F4-98F5-AAEC25ECACBE}" name="bg_clr" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{767B200D-BA70-439B-94A5-74CB8576CAA0}" name="bg_bri" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{3986F5DC-2BA5-44B0-A8F4-7A7ACEA7BCB1}" name="this_fade" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{735AEADE-E42C-40CD-BC0F-2BDDEB978719}" name="Table9" displayName="Table9" ref="B3:F12" totalsRowShown="0">
-  <autoFilter ref="B3:F12" xr:uid="{2D982AFB-B968-492E-BD67-697A4FE341EE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{735AEADE-E42C-40CD-BC0F-2BDDEB978719}" name="Table9" displayName="Table9" ref="B3:F20" totalsRowShown="0">
+  <autoFilter ref="B3:F20" xr:uid="{2D982AFB-B968-492E-BD67-697A4FE341EE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{05A310C9-4A29-45A4-A606-C9DC5B7D6B21}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{B86BD539-A9BB-4562-B337-63A65AFC3C27}" name="scale"/>
-    <tableColumn id="5" xr3:uid="{6FBF2B45-6040-4C57-8C81-047AEF6F64B5}" name="scale2"/>
-    <tableColumn id="3" xr3:uid="{FF203808-A99F-4790-96DC-2E7465E0BAE0}" name="this_delay"/>
-    <tableColumn id="4" xr3:uid="{765884F8-5D09-4A63-AA45-9522233E62C7}" name="target_palette"/>
+    <tableColumn id="2" xr3:uid="{B86BD539-A9BB-4562-B337-63A65AFC3C27}" name="scale" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{6FBF2B45-6040-4C57-8C81-047AEF6F64B5}" name="scale2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FF203808-A99F-4790-96DC-2E7465E0BAE0}" name="this_delay" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{765884F8-5D09-4A63-AA45-9522233E62C7}" name="target_palette" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1148,19 +1169,19 @@
   <autoFilter ref="C5:P44" xr:uid="{33006C65-6254-4C2E-BA90-A793C18B517B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{D451EFD4-08DE-4D68-937A-6BDCEE1F682A}" name="mode"/>
-    <tableColumn id="3" xr3:uid="{5883A58A-20CA-4E81-9909-A6F77A954824}" name="spiral_width" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{EA20131A-2FB1-42DC-92E8-009F201A0E4C}" name="spiral_inc" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{A18CF2BF-B2C4-463D-B6BB-86282AEAFC90}" name="this_hue" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{8ED8F96E-9098-46A4-BBCF-5EE841CEC53F}" name="this_inc" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{681C7FB6-894A-4108-9431-D245BAD61DF9}" name="this_speed" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{7F663E86-311B-4734-8584-41CD18ADB568}" name="this_rot" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{AF455D61-496F-4E9A-A0C7-FEDCFFC00113}" name="all_freq" dataDxfId="24"/>
-    <tableColumn id="14" xr3:uid="{D6F6226B-3E30-45FE-8738-A77C384B7AF2}" name="that_speed" dataDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{F283AB4A-2A73-41AA-9846-39CADFA4CD34}" name="Column2" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{2744D8B9-518B-47BA-BD49-B78AF6AB55C7}" name="bg_clr" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{A97EB7F3-7BB6-4B29-AB05-0DEA7C7B8FC1}" name="bg_bri" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{587FCE08-EEBE-4135-BAB3-49DAC525E1F1}" name="this_delay" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{03095349-BD0F-45EA-90E9-5472A41B7E6B}" name="target_palette" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{5883A58A-20CA-4E81-9909-A6F77A954824}" name="spiral_width" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{EA20131A-2FB1-42DC-92E8-009F201A0E4C}" name="spiral_inc" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{A18CF2BF-B2C4-463D-B6BB-86282AEAFC90}" name="this_hue" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{8ED8F96E-9098-46A4-BBCF-5EE841CEC53F}" name="this_inc" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{681C7FB6-894A-4108-9431-D245BAD61DF9}" name="this_speed" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{7F663E86-311B-4734-8584-41CD18ADB568}" name="this_rot" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{AF455D61-496F-4E9A-A0C7-FEDCFFC00113}" name="all_freq" dataDxfId="28"/>
+    <tableColumn id="14" xr3:uid="{D6F6226B-3E30-45FE-8738-A77C384B7AF2}" name="that_speed" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{F283AB4A-2A73-41AA-9846-39CADFA4CD34}" name="Column2" dataDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{2744D8B9-518B-47BA-BD49-B78AF6AB55C7}" name="bg_clr" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{A97EB7F3-7BB6-4B29-AB05-0DEA7C7B8FC1}" name="bg_bri" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{587FCE08-EEBE-4135-BAB3-49DAC525E1F1}" name="this_delay" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{03095349-BD0F-45EA-90E9-5472A41B7E6B}" name="target_palette" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1188,14 +1209,14 @@
   <autoFilter ref="C5:K13" xr:uid="{647C1886-CAF5-4AD0-935B-332451C9BA78}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A92C0E86-03FD-40DC-91DC-DEF026246354}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{2200EF9C-1450-4853-9AE5-56B41D1F69B8}" name="mul1" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{EF161261-B5EF-4532-A702-979022B37225}" name="mul2" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{DCC1E6A5-1978-4D3D-9D67-596C69ADAEEF}" name="mul3" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{1B829B8C-B435-423A-BB43-30BD398472D2}" name="mul1r" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{5B81F7A2-5C96-4FD2-A49A-84321424C70D}" name="mul2r" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{4486FCB4-072B-4B6B-ABB3-D116B4FA0D0F}" name="mul3r" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{33F25931-6A37-470C-A20E-100ADAE31FE1}" name="this_delay" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{8A7A7265-B42D-4D3E-8DA9-BF829F5D12BF}" name="target_palette" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{2200EF9C-1450-4853-9AE5-56B41D1F69B8}" name="mul1" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{EF161261-B5EF-4532-A702-979022B37225}" name="mul2" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{DCC1E6A5-1978-4D3D-9D67-596C69ADAEEF}" name="mul3" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{1B829B8C-B435-423A-BB43-30BD398472D2}" name="mul1r" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{5B81F7A2-5C96-4FD2-A49A-84321424C70D}" name="mul2r" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{4486FCB4-072B-4B6B-ABB3-D116B4FA0D0F}" name="mul3r" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{33F25931-6A37-470C-A20E-100ADAE31FE1}" name="this_delay" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{8A7A7265-B42D-4D3E-8DA9-BF829F5D12BF}" name="target_palette" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1220,16 +1241,16 @@
   <autoFilter ref="C4:M19" xr:uid="{EE3E795F-5D4E-4DF2-909E-0D1BCBB1D820}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{57E55E03-80DB-401D-A6F8-3837F87C4FF6}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{72139E1C-36E1-4E8D-A419-1A9D5E19B27B}" name="this_speed" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{C4CBAF6C-6A4A-4A94-BF41-A54D2049DBDD}" name="that_speed" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{E728F420-E8EA-469A-9FD8-DF954D0605C4}" name="this_rot" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{DE575798-DF59-4E2B-9B0D-4DDE05C224F9}" name="that_rot" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{62BB0B40-5043-4AE5-93B2-B4BC494EB388}" name="all_freq" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{384979C4-E3C7-4861-BEE1-3E901C9B5D8C}" name="this_cutoff" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{B7CD300C-57CE-47E4-958A-D9F134C93B41}" name="that_cutoff" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{920AF0E4-3D55-4CB5-8776-852DC53901B1}" name="this_sat" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{0F87F6FA-5922-4755-ADAC-315EA1E24339}" name="this_delay" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{56537C11-EAD3-4C35-A4A6-AD8FC54CDF55}" name="target_palette" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{72139E1C-36E1-4E8D-A419-1A9D5E19B27B}" name="this_speed" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{C4CBAF6C-6A4A-4A94-BF41-A54D2049DBDD}" name="that_speed" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{E728F420-E8EA-469A-9FD8-DF954D0605C4}" name="this_rot" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{DE575798-DF59-4E2B-9B0D-4DDE05C224F9}" name="that_rot" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{62BB0B40-5043-4AE5-93B2-B4BC494EB388}" name="all_freq" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{384979C4-E3C7-4861-BEE1-3E901C9B5D8C}" name="this_cutoff" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{B7CD300C-57CE-47E4-958A-D9F134C93B41}" name="that_cutoff" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{920AF0E4-3D55-4CB5-8776-852DC53901B1}" name="this_sat" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{0F87F6FA-5922-4755-ADAC-315EA1E24339}" name="this_delay" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{56537C11-EAD3-4C35-A4A6-AD8FC54CDF55}" name="target_palette" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1322,18 +1343,18 @@
   <autoFilter ref="B3:N44" xr:uid="{BC983D0E-72F1-46A6-A34F-0D3115A13C31}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8A06A4F3-45AF-4652-B223-BDB11410A52A}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{D5CF372E-8371-4313-8740-2944A4CF04C2}" name="juggle_index_reset" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{4C0F5AD5-FBAA-40BC-9F56-6E1DFEA16438}" name="this_fade" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{0C1DE2B9-A77C-4E60-9D7C-DC2CE31F17A1}" name="numdots_ring" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{8AE921B7-CB65-4227-AE7E-CEF139D70EDE}" name="numdots" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{A9D85CDA-C3C6-44D3-8076-75E3B2DA3C14}" name="this_beat" dataDxfId="44"/>
-    <tableColumn id="13" xr3:uid="{870F8A55-34BE-4730-BC78-F6218FF582B6}" name="ringBeat" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{50949DD2-3C68-4AB3-84C4-95C3335C1C0F}" name="this_diff" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{38F98679-ED7F-424F-A584-FFFAC335C341}" name="target_palette" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{F55D081A-A571-4732-8962-5670EDC4BAE7}" name="this_delay" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{1B108AAB-822A-4AAB-9969-62D73DFE8D9F}" name="cooling1-4" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{CC4AAF48-640F-4A6A-9335-F7696968A79B}" name="sparking1-4" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{BB67BBB9-C1D0-44B5-9EEE-EADD648958AA}" name="Notes" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{D5CF372E-8371-4313-8740-2944A4CF04C2}" name="juggle_index_reset" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{4C0F5AD5-FBAA-40BC-9F56-6E1DFEA16438}" name="this_fade" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{0C1DE2B9-A77C-4E60-9D7C-DC2CE31F17A1}" name="numdots_ring" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{8AE921B7-CB65-4227-AE7E-CEF139D70EDE}" name="numdots" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{A9D85CDA-C3C6-44D3-8076-75E3B2DA3C14}" name="this_beat" dataDxfId="48"/>
+    <tableColumn id="13" xr3:uid="{870F8A55-34BE-4730-BC78-F6218FF582B6}" name="ringBeat" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{50949DD2-3C68-4AB3-84C4-95C3335C1C0F}" name="this_diff" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{38F98679-ED7F-424F-A584-FFFAC335C341}" name="target_palette" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{F55D081A-A571-4732-8962-5670EDC4BAE7}" name="this_delay" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{1B108AAB-822A-4AAB-9969-62D73DFE8D9F}" name="cooling1-4" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{CC4AAF48-640F-4A6A-9335-F7696968A79B}" name="sparking1-4" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{BB67BBB9-C1D0-44B5-9EEE-EADD648958AA}" name="jug16_phase" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1641,8 +1662,8 @@
   </sheetPr>
   <dimension ref="B4:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,6 +2188,12 @@
       </c>
       <c r="C24" t="s">
         <v>101</v>
+      </c>
+      <c r="D24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
       </c>
       <c r="G24" s="9">
         <v>116</v>
@@ -2551,10 +2578,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558A69EF-C943-41AA-AE07-FFE240D8DD82}">
-  <dimension ref="A3:F12"/>
+  <dimension ref="A3:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,16 +2630,28 @@
       <c r="B5" t="s">
         <v>135</v>
       </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>135</v>
       </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>135</v>
       </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -2636,21 +2675,131 @@
       <c r="B9" t="s">
         <v>136</v>
       </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>136</v>
       </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>136</v>
       </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>136</v>
       </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4371,7 +4520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77779BD-95B5-4C4A-BC04-7BB2350DA5C2}">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -5771,8 +5920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298B5153-BF4C-4682-9BCF-06258537994F}">
   <dimension ref="A3:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5789,6 +5938,7 @@
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -5829,7 +5979,7 @@
         <v>121</v>
       </c>
       <c r="N3" t="s">
-        <v>112</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6621,7 +6771,9 @@
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
+      <c r="N41" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="15">

</xml_diff>

<commit_message>
and the keyboard excel file
</commit_message>
<xml_diff>
--- a/readkeyboard_options.xlsx
+++ b/readkeyboard_options.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeffKarle\Documents\cinder_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC402276-D147-4803-9C21-A6E0BED2FCD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27615" yWindow="3870" windowWidth="18375" windowHeight="7830" firstSheet="17" activeTab="19"/>
+    <workbookView xWindow="-36225" yWindow="4110" windowWidth="18375" windowHeight="15885" tabRatio="765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keyboard" sheetId="1" r:id="rId1"/>
@@ -22,11 +23,11 @@
     <sheet name="fire" sheetId="7" r:id="rId8"/>
     <sheet name="juggle" sheetId="6" r:id="rId9"/>
     <sheet name="matrix" sheetId="17" r:id="rId10"/>
-    <sheet name="noise8" sheetId="8" r:id="rId11"/>
-    <sheet name="one_sin" sheetId="9" r:id="rId12"/>
-    <sheet name="plasma" sheetId="10" r:id="rId13"/>
-    <sheet name="rainbow_march" sheetId="11" r:id="rId14"/>
-    <sheet name="Sheet1" sheetId="21" r:id="rId15"/>
+    <sheet name="movingdot" sheetId="21" r:id="rId11"/>
+    <sheet name="noise8" sheetId="8" r:id="rId12"/>
+    <sheet name="one_sin" sheetId="9" r:id="rId13"/>
+    <sheet name="plasma" sheetId="10" r:id="rId14"/>
+    <sheet name="rainbow_march" sheetId="11" r:id="rId15"/>
     <sheet name="ripple" sheetId="12" r:id="rId16"/>
     <sheet name="serendipitous" sheetId="13" r:id="rId17"/>
     <sheet name="spiral" sheetId="14" r:id="rId18"/>
@@ -39,18 +40,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="217">
   <si>
     <t>letter</t>
   </si>
@@ -193,9 +188,6 @@
     <t>u</t>
   </si>
   <si>
-    <t>this_bright</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
@@ -541,15 +533,6 @@
     <t>mul3</t>
   </si>
   <si>
-    <t>mul123r</t>
-  </si>
-  <si>
-    <t>[0-2][0-255]</t>
-  </si>
-  <si>
-    <t>mul123</t>
-  </si>
-  <si>
     <t>E1</t>
   </si>
   <si>
@@ -652,9 +635,6 @@
     <t>fade_rainbow</t>
   </si>
   <si>
-    <t>float</t>
-  </si>
-  <si>
     <t>matrix_ray</t>
   </si>
   <si>
@@ -686,12 +666,42 @@
   </si>
   <si>
     <t>D2</t>
+  </si>
+  <si>
+    <t>movingdot</t>
+  </si>
+  <si>
+    <t>blue_angle</t>
+  </si>
+  <si>
+    <t>blue_low</t>
+  </si>
+  <si>
+    <t>blue_high</t>
+  </si>
+  <si>
+    <t>green_angle</t>
+  </si>
+  <si>
+    <t>green_low</t>
+  </si>
+  <si>
+    <t>green_high</t>
+  </si>
+  <si>
+    <t>red_angle</t>
+  </si>
+  <si>
+    <t>red_low</t>
+  </si>
+  <si>
+    <t>red_high</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,7 +899,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="65">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1066,311 +1109,332 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:E30" totalsRowShown="0">
-  <autoFilter ref="B4:E30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B4:E30" totalsRowShown="0">
+  <autoFilter ref="B4:E30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ascii "/>
-    <tableColumn id="2" name="letter"/>
-    <tableColumn id="3" name="variable"/>
-    <tableColumn id="4" name="range"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ascii "/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="letter"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="variable"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="range"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="C4:I18" totalsRowShown="0">
-  <autoFilter ref="C4:I18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table16" displayName="Table16" ref="C4:I18" totalsRowShown="0">
+  <autoFilter ref="C4:I18" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_rot" dataDxfId="41"/>
-    <tableColumn id="3" name="this_delay" dataDxfId="40"/>
-    <tableColumn id="4" name="target_palette" dataDxfId="39"/>
-    <tableColumn id="5" name="bg_clr" dataDxfId="38"/>
-    <tableColumn id="6" name="bg_bri" dataDxfId="37"/>
-    <tableColumn id="7" name="this_fade" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="this_rot" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="this_delay" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="target_palette" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="bg_clr" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="bg_bri" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="this_fade" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="B3:G20" totalsRowShown="0">
-  <autoFilter ref="B3:G20"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="scale" dataDxfId="35"/>
-    <tableColumn id="5" name="scale2" dataDxfId="34"/>
-    <tableColumn id="3" name="this_delay" dataDxfId="33"/>
-    <tableColumn id="4" name="target_palette" dataDxfId="32"/>
-    <tableColumn id="6" name="Column1" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7CB80328-1019-4BD3-A3E2-F82C00C0D67D}" name="Table21" displayName="Table21" ref="B5:M11" totalsRowShown="0">
+  <autoFilter ref="B5:M11" xr:uid="{1043DD12-DC60-4826-A91B-624EE2E4AABD}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{40FE2BF6-1002-4F74-900E-52B6D9F0770D}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{90554CB9-5D07-493B-ADFF-C68636D678F0}" name="this_fade" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{DA85B59B-1E9F-4E9A-BD6B-E67C21387976}" name="this_delay" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A890E05A-E6F5-4F1D-94C3-2F4B6245D062}" name="blue_angle" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{D9859800-95AE-4CAB-AFFB-1986A1C93215}" name="blue_low" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{83A21592-77A7-4226-BA18-5469CA3235BD}" name="blue_high" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{180F7B8E-35E6-480C-9EDB-F01CDC23A6F5}" name="green_angle" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{B1D7A590-028F-43CF-B941-90F97FDD535A}" name="green_low" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{72756E36-653C-4D62-BD21-9DAF3BCAD1CC}" name="green_high" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{7E44ED25-019D-4EEF-A458-51627270C66C}" name="red_angle" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{0687BB42-C6CB-4C9E-9497-66B8BF6FBC45}" name="red_low" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{29C4DA03-C1FF-41DA-9B25-B19782499507}" name="red_high" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="C4:L14" totalsRowShown="0">
-  <autoFilter ref="C4:L14"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_inc"/>
-    <tableColumn id="3" name="this_speed"/>
-    <tableColumn id="4" name="all_freq"/>
-    <tableColumn id="5" name="this_cutoff"/>
-    <tableColumn id="6" name="bg_clr"/>
-    <tableColumn id="7" name="bg_bri"/>
-    <tableColumn id="8" name="this_rot"/>
-    <tableColumn id="9" name="this_delay"/>
-    <tableColumn id="10" name="target_palette"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table9" displayName="Table9" ref="B3:G20" totalsRowShown="0">
+  <autoFilter ref="B3:G20" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="scale" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="scale2" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="this_delay" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="target_palette" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Column1" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="C4:E9" totalsRowShown="0">
-  <autoFilter ref="C4:E9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table10" displayName="Table10" ref="C4:L14" totalsRowShown="0">
+  <autoFilter ref="C4:L14" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="this_inc"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="this_speed"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="all_freq"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="this_cutoff"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="bg_clr"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="bg_bri"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="this_rot"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0B00-000009000000}" name="this_delay"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0B00-00000A000000}" name="target_palette"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table11" displayName="Table11" ref="C4:E9" totalsRowShown="0">
+  <autoFilter ref="C4:E9" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_delay"/>
-    <tableColumn id="3" name="target_palette"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="this_delay"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="target_palette"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="C4:F16" totalsRowShown="0">
-  <autoFilter ref="C4:F16"/>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table12" displayName="Table12" ref="C4:F16" totalsRowShown="0">
+  <autoFilter ref="C4:F16" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_rot"/>
-    <tableColumn id="3" name="this_diff"/>
-    <tableColumn id="4" name="this_delay"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C4:G10" totalsRowShown="0">
-  <autoFilter ref="C4:G10"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_fade"/>
-    <tableColumn id="3" name="this_delay"/>
-    <tableColumn id="4" name="target_palette"/>
-    <tableColumn id="5" name="myfade"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="this_rot"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="this_diff"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="this_delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="C4:F13" totalsRowShown="0">
-  <autoFilter ref="C4:F13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table2" displayName="Table2" ref="C4:G10" totalsRowShown="0">
+  <autoFilter ref="C4:G10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="this_fade"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="this_delay"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="target_palette"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="myfade"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table13" displayName="Table13" ref="C4:F13" totalsRowShown="0">
+  <autoFilter ref="C4:F13" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_delay"/>
-    <tableColumn id="3" name="target_palette"/>
-    <tableColumn id="4" name="this_fade"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="this_delay"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="target_palette"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="this_fade"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="C5:P44" totalsRowShown="0">
-  <autoFilter ref="C5:P44"/>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table14" displayName="Table14" ref="C5:P44" totalsRowShown="0">
+  <autoFilter ref="C5:P44" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="3" name="spiral_width" dataDxfId="31"/>
-    <tableColumn id="6" name="spiral_inc" dataDxfId="30"/>
-    <tableColumn id="4" name="this_hue" dataDxfId="29"/>
-    <tableColumn id="8" name="this_inc" dataDxfId="28"/>
-    <tableColumn id="9" name="this_speed" dataDxfId="27"/>
-    <tableColumn id="10" name="this_rot" dataDxfId="26"/>
-    <tableColumn id="11" name="all_freq" dataDxfId="25"/>
-    <tableColumn id="14" name="that_speed" dataDxfId="24"/>
-    <tableColumn id="15" name="Column2" dataDxfId="23"/>
-    <tableColumn id="12" name="bg_clr" dataDxfId="22"/>
-    <tableColumn id="13" name="bg_bri" dataDxfId="21"/>
-    <tableColumn id="5" name="this_delay" dataDxfId="20"/>
-    <tableColumn id="7" name="target_palette" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="mode"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="spiral_width" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="spiral_inc" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="this_hue" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1000-000008000000}" name="this_inc" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1000-000009000000}" name="this_speed" dataDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1000-00000A000000}" name="this_rot" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1000-00000B000000}" name="all_freq" dataDxfId="35"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1000-00000E000000}" name="that_speed" dataDxfId="34"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1000-00000F000000}" name="Column2" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1000-00000C000000}" name="bg_clr" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1000-00000D000000}" name="bg_bri" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="this_delay" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="target_palette" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="C3:J6" totalsRowShown="0">
-  <autoFilter ref="C3:J6"/>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table19" displayName="Table19" ref="C3:J6" totalsRowShown="0">
+  <autoFilter ref="C3:J6" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="twinkle_speed"/>
-    <tableColumn id="3" name="twinkle_density"/>
-    <tableColumn id="4" name="twinkle_bg"/>
-    <tableColumn id="5" name="auto_select_background_color"/>
-    <tableColumn id="7" name="cool_like_incandescent"/>
-    <tableColumn id="8" name="this_delay"/>
-    <tableColumn id="9" name="target_palette"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="twinkle_speed"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="twinkle_density"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="twinkle_bg"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="auto_select_background_color"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="cool_like_incandescent"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="this_delay"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1100-000009000000}" name="target_palette"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="C5:K13" totalsRowShown="0">
-  <autoFilter ref="C5:K13"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="mul1" dataDxfId="18"/>
-    <tableColumn id="3" name="mul2" dataDxfId="17"/>
-    <tableColumn id="4" name="mul3" dataDxfId="16"/>
-    <tableColumn id="7" name="mul1r" dataDxfId="15"/>
-    <tableColumn id="8" name="mul2r" dataDxfId="14"/>
-    <tableColumn id="9" name="mul3r" dataDxfId="13"/>
-    <tableColumn id="5" name="this_delay" dataDxfId="12"/>
-    <tableColumn id="6" name="target_palette" dataDxfId="11"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:F18" totalsRowShown="0">
-  <autoFilter ref="B3:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="B3:F18" totalsRowShown="0">
+  <autoFilter ref="B3:F18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_fade"/>
-    <tableColumn id="3" name="vImpact0"/>
-    <tableColumn id="4" name="target_palette"/>
-    <tableColumn id="5" name="this_delay"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="this_fade"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="vImpact0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="target_palette"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="this_delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="C4:M19" totalsRowShown="0">
-  <autoFilter ref="C4:M19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table15" displayName="Table15" ref="C5:K13" totalsRowShown="0">
+  <autoFilter ref="C5:K13" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="mul1" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="mul2" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="mul3" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="mul1r" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1200-000008000000}" name="mul2r" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1200-000009000000}" name="mul3r" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="this_delay" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="target_palette" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table17" displayName="Table17" ref="C4:M19" totalsRowShown="0">
+  <autoFilter ref="C4:M19" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_speed" dataDxfId="10"/>
-    <tableColumn id="3" name="that_speed" dataDxfId="9"/>
-    <tableColumn id="4" name="this_rot" dataDxfId="8"/>
-    <tableColumn id="5" name="that_rot" dataDxfId="7"/>
-    <tableColumn id="6" name="all_freq" dataDxfId="6"/>
-    <tableColumn id="8" name="this_cutoff" dataDxfId="5"/>
-    <tableColumn id="9" name="that_cutoff" dataDxfId="4"/>
-    <tableColumn id="10" name="this_sat" dataDxfId="3"/>
-    <tableColumn id="11" name="this_delay" dataDxfId="2"/>
-    <tableColumn id="12" name="target_palette" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="this_speed" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="that_speed" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="this_rot" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="that_rot" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1300-000006000000}" name="all_freq" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1300-000008000000}" name="this_cutoff" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1300-000009000000}" name="that_cutoff" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1300-00000A000000}" name="this_sat" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1300-00000B000000}" name="this_delay" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1300-00000C000000}" name="target_palette" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B4:F24" totalsRowShown="0">
-  <autoFilter ref="B4:F24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="B4:F24" totalsRowShown="0">
+  <autoFilter ref="B4:F24" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="scale"/>
-    <tableColumn id="3" name="target_palette"/>
-    <tableColumn id="5" name="this_delay"/>
-    <tableColumn id="4" name="Notes"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="scale"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="target_palette"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="this_delay"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B3:D10" totalsRowShown="0">
-  <autoFilter ref="B3:D10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="B3:D10" totalsRowShown="0">
+  <autoFilter ref="B3:D10" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="target_palette"/>
-    <tableColumn id="3" name="this_delay"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="target_palette"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="this_delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="B4:D8" totalsRowShown="0">
-  <autoFilter ref="B4:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table20" displayName="Table20" ref="B4:D8" totalsRowShown="0">
+  <autoFilter ref="B4:D8" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_delay "/>
-    <tableColumn id="3" name="target_palette"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="this_delay "/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="target_palette"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B3:H9" totalsRowShown="0">
-  <autoFilter ref="B3:H9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="B3:H9" totalsRowShown="0">
+  <autoFilter ref="B3:H9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_diff"/>
-    <tableColumn id="3" name="this_inc"/>
-    <tableColumn id="7" name="this_fade"/>
-    <tableColumn id="4" name="target_palette"/>
-    <tableColumn id="5" name="this_delay"/>
-    <tableColumn id="6" name="Notes"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="this_diff"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="this_inc"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="this_fade"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="target_palette"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="this_delay"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="C4:E12" totalsRowShown="0">
-  <autoFilter ref="C4:E12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table18" displayName="Table18" ref="C4:E12" totalsRowShown="0">
+  <autoFilter ref="C4:E12" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="this_hue"/>
-    <tableColumn id="3" name="this_delay"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="this_hue"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="this_delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:H40" totalsRowShown="0">
-  <autoFilter ref="B3:H40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table8" displayName="Table8" ref="B3:H40" totalsRowShown="0">
+  <autoFilter ref="B3:H40" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="cooling"/>
-    <tableColumn id="3" name="sparking"/>
-    <tableColumn id="4" name="this_delay"/>
-    <tableColumn id="5" name="target_palette"/>
-    <tableColumn id="6" name="cooling1-4"/>
-    <tableColumn id="7" name="sparking1-4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="cooling"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="sparking"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="this_delay"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="target_palette"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="cooling1-4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="sparking1-4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:N44" totalsRowShown="0">
-  <autoFilter ref="B3:N44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table7" displayName="Table7" ref="B3:N44" totalsRowShown="0">
+  <autoFilter ref="B3:N44" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="mode"/>
-    <tableColumn id="2" name="juggle_index_reset" dataDxfId="53"/>
-    <tableColumn id="3" name="this_fade" dataDxfId="52"/>
-    <tableColumn id="4" name="numdots_ring" dataDxfId="51"/>
-    <tableColumn id="12" name="numdots" dataDxfId="50"/>
-    <tableColumn id="5" name="this_beat" dataDxfId="49"/>
-    <tableColumn id="13" name="ringBeat" dataDxfId="48"/>
-    <tableColumn id="6" name="this_diff" dataDxfId="47"/>
-    <tableColumn id="7" name="target_palette" dataDxfId="46"/>
-    <tableColumn id="8" name="this_delay" dataDxfId="45"/>
-    <tableColumn id="11" name="cooling1-4" dataDxfId="44"/>
-    <tableColumn id="10" name="sparking1-4" dataDxfId="43"/>
-    <tableColumn id="9" name="jug16_phase" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="mode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="juggle_index_reset" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="this_fade" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="numdots_ring" dataDxfId="62"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="numdots" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="this_beat" dataDxfId="60"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="ringBeat" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="this_diff" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="target_palette" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="this_delay" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="cooling1-4" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="sparking1-4" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="jug16_phase" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1672,14 +1736,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B4:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,10 +1789,10 @@
         <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1740,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>7</v>
@@ -1751,10 +1815,10 @@
         <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -1777,25 +1841,25 @@
         <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G7" s="6">
         <v>99</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -1803,13 +1867,13 @@
         <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>164</v>
+        <v>7</v>
       </c>
       <c r="G8" s="9">
         <v>100</v>
@@ -1829,13 +1893,13 @@
         <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E9" t="s">
-        <v>164</v>
+        <v>7</v>
       </c>
       <c r="G9" s="6">
         <v>101</v>
@@ -1851,7 +1915,13 @@
         <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
       </c>
       <c r="G10" s="9">
         <v>102</v>
@@ -1871,10 +1941,10 @@
         <v>71</v>
       </c>
       <c r="C11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
         <v>90</v>
-      </c>
-      <c r="D11" t="s">
-        <v>91</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -1897,10 +1967,10 @@
         <v>72</v>
       </c>
       <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" t="s">
         <v>92</v>
-      </c>
-      <c r="D12" t="s">
-        <v>93</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -1923,13 +1993,13 @@
         <v>73</v>
       </c>
       <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
         <v>94</v>
       </c>
-      <c r="D13" t="s">
-        <v>95</v>
-      </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="6">
         <v>105</v>
@@ -1949,10 +2019,10 @@
         <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1975,10 +2045,10 @@
         <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -2001,10 +2071,10 @@
         <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -2027,10 +2097,10 @@
         <v>77</v>
       </c>
       <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" t="s">
         <v>80</v>
-      </c>
-      <c r="D17" t="s">
-        <v>81</v>
       </c>
       <c r="G17" s="6">
         <v>109</v>
@@ -2050,13 +2120,13 @@
         <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G18" s="9">
         <v>110</v>
@@ -2065,7 +2135,7 @@
         <v>32</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>7</v>
@@ -2076,10 +2146,10 @@
         <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -2102,10 +2172,10 @@
         <v>80</v>
       </c>
       <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
         <v>82</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
       </c>
       <c r="G20" s="9">
         <v>112</v>
@@ -2125,13 +2195,13 @@
         <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" t="s">
         <v>129</v>
-      </c>
-      <c r="E21" t="s">
-        <v>130</v>
       </c>
       <c r="G21" s="6">
         <v>113</v>
@@ -2151,10 +2221,10 @@
         <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
@@ -2177,13 +2247,13 @@
         <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G23" s="6">
         <v>115</v>
@@ -2203,13 +2273,13 @@
         <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G24" s="9">
         <v>116</v>
@@ -2229,7 +2299,13 @@
         <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
       </c>
       <c r="G25" s="6">
         <v>117</v>
@@ -2238,7 +2314,7 @@
         <v>46</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>7</v>
@@ -2249,22 +2325,22 @@
         <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>209</v>
       </c>
       <c r="E26" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="G26" s="9">
         <v>118</v>
       </c>
       <c r="H26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>7</v>
@@ -2275,16 +2351,22 @@
         <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="D27" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
       </c>
       <c r="G27" s="6">
         <v>119</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J27" s="8"/>
     </row>
@@ -2293,13 +2375,19 @@
         <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="D28" t="s">
+        <v>211</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
       </c>
       <c r="G28" s="9">
         <v>120</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>33</v>
@@ -2313,32 +2401,52 @@
         <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="D29" t="s">
+        <v>212</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
       </c>
       <c r="G29" s="6">
         <v>121</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="8"/>
+        <v>53</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>213</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
       </c>
       <c r="G30" s="12">
         <v>122</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="14"/>
+        <v>55</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2350,7 +2458,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B4:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2367,7 +2475,7 @@
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -2379,10 +2487,10 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
         <v>35</v>
@@ -2402,10 +2510,10 @@
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>34</v>
@@ -2416,7 +2524,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2427,7 +2535,7 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2438,7 +2546,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2471,7 +2579,7 @@
         <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2482,7 +2590,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2493,7 +2601,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2524,7 +2632,7 @@
         <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2535,7 +2643,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2564,7 +2672,7 @@
         <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2575,7 +2683,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2593,7 +2701,180 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A5:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" t="s">
+        <v>210</v>
+      </c>
+      <c r="H5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I5" t="s">
+        <v>212</v>
+      </c>
+      <c r="J5" t="s">
+        <v>213</v>
+      </c>
+      <c r="K5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L5" t="s">
+        <v>215</v>
+      </c>
+      <c r="M5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A3:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2609,13 +2890,13 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -2624,7 +2905,7 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2632,7 +2913,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
@@ -2648,7 +2929,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -2658,7 +2939,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -2668,7 +2949,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2682,7 +2963,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
@@ -2694,10 +2975,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2707,7 +2988,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2717,7 +2998,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2727,7 +3008,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2740,10 +3021,10 @@
         <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
@@ -2758,7 +3039,7 @@
         <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2768,7 +3049,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2778,7 +3059,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2791,10 +3072,10 @@
         <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
@@ -2809,7 +3090,7 @@
         <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -2824,12 +3105,12 @@
         <v>27</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2839,7 +3120,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2855,8 +3136,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B4:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2877,7 +3158,7 @@
   <sheetData>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -2892,10 +3173,10 @@
         <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J4" t="s">
         <v>29</v>
@@ -2918,16 +3199,16 @@
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>28</v>
@@ -2944,22 +3225,22 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -2973,16 +3254,16 @@
         <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>28</v>
@@ -2996,25 +3277,25 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3025,8 +3306,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="B4:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3041,7 +3322,7 @@
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -3066,22 +3347,22 @@
         <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3092,8 +3373,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="B4:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3110,7 +3391,7 @@
   <sheetData>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -3138,20 +3419,20 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -3170,20 +3451,20 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -3199,17 +3480,17 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3220,20 +3501,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="B4:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3250,7 +3519,7 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
@@ -3262,7 +3531,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -3279,7 +3548,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -3287,27 +3556,27 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3319,7 +3588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="B4:F13"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -3336,7 +3605,7 @@
   <sheetData>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -3367,22 +3636,22 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -3390,22 +3659,22 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3417,7 +3686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="B5:Q44"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -3442,13 +3711,13 @@
   <sheetData>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
@@ -3466,16 +3735,16 @@
         <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O5" t="s">
         <v>11</v>
@@ -3489,10 +3758,10 @@
         <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>20</v>
@@ -3515,7 +3784,7 @@
         <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -3533,7 +3802,7 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -3551,7 +3820,7 @@
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -3569,7 +3838,7 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -3590,10 +3859,10 @@
         <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>20</v>
@@ -3612,7 +3881,7 @@
         <v>10</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q11" s="1"/>
     </row>
@@ -3621,7 +3890,7 @@
         <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -3639,7 +3908,7 @@
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3657,7 +3926,7 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3690,7 +3959,7 @@
         <v>28</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -3700,7 +3969,7 @@
         <v>10</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
@@ -3708,7 +3977,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -3726,7 +3995,7 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3744,7 +4013,7 @@
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3762,7 +4031,7 @@
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3795,7 +4064,7 @@
         <v>28</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -3805,7 +4074,7 @@
         <v>10</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -3813,7 +4082,7 @@
         <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -3831,7 +4100,7 @@
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -3849,7 +4118,7 @@
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -3882,7 +4151,7 @@
         <v>28</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -3892,7 +4161,7 @@
         <v>10</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
@@ -3900,7 +4169,7 @@
         <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3918,7 +4187,7 @@
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -3936,7 +4205,7 @@
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -3954,7 +4223,7 @@
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -3987,23 +4256,23 @@
         <v>28</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
@@ -4011,7 +4280,7 @@
         <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -4029,7 +4298,7 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -4047,7 +4316,7 @@
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -4082,7 +4351,7 @@
         <v>10</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
@@ -4090,7 +4359,7 @@
         <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -4108,7 +4377,7 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -4126,7 +4395,7 @@
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -4161,7 +4430,7 @@
         <v>10</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -4169,7 +4438,7 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -4187,7 +4456,7 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -4205,7 +4474,7 @@
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -4244,7 +4513,7 @@
         <v>10</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
@@ -4252,7 +4521,7 @@
         <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -4270,7 +4539,7 @@
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -4288,7 +4557,7 @@
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -4314,7 +4583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="B3:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4334,22 +4603,22 @@
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H3" t="s">
         <v>187</v>
-      </c>
-      <c r="E3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H3" t="s">
-        <v>191</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -4374,12 +4643,12 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -4391,7 +4660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4412,7 +4681,7 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -4420,13 +4689,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -4443,7 +4712,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -4457,7 +4726,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -4468,7 +4737,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6">
         <v>32</v>
@@ -4477,12 +4746,12 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -4493,7 +4762,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
@@ -4501,7 +4770,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
@@ -4509,7 +4778,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" t="s">
         <v>19</v>
@@ -4520,10 +4789,10 @@
         <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -4537,7 +4806,7 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -4551,7 +4820,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E13">
         <v>44</v>
@@ -4559,27 +4828,27 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4591,10 +4860,10 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="B5:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -4608,25 +4877,25 @@
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
         <v>160</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>161</v>
       </c>
-      <c r="F5" t="s">
-        <v>162</v>
-      </c>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
@@ -4640,13 +4909,13 @@
         <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -4663,7 +4932,7 @@
         <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -4676,7 +4945,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -4689,7 +4958,7 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -4708,13 +4977,13 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>10</v>
@@ -4725,10 +4994,10 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -4741,7 +5010,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -4754,7 +5023,7 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -4775,7 +5044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="B4:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4800,19 +5069,19 @@
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -4821,7 +5090,7 @@
         <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K4" t="s">
         <v>43</v>
@@ -4841,22 +5110,22 @@
         <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>42</v>
@@ -4868,10 +5137,10 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -4886,7 +5155,7 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -4901,7 +5170,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -4916,7 +5185,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -4937,22 +5206,22 @@
         <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>42</v>
@@ -4964,10 +5233,10 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -4982,7 +5251,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -4997,7 +5266,7 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -5012,7 +5281,7 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -5033,22 +5302,22 @@
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
@@ -5063,7 +5332,7 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -5078,7 +5347,7 @@
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -5093,7 +5362,7 @@
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5108,7 +5377,7 @@
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5130,7 +5399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A4:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5147,10 +5416,10 @@
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -5159,7 +5428,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5167,7 +5436,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
@@ -5181,33 +5450,33 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -5215,7 +5484,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
@@ -5227,27 +5496,27 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -5267,7 +5536,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -5276,12 +5545,12 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -5300,17 +5569,17 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -5322,7 +5591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5338,7 +5607,7 @@
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -5363,32 +5632,32 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -5400,7 +5669,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5415,10 +5684,10 @@
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -5437,17 +5706,17 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -5459,7 +5728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A3:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5478,7 +5747,7 @@
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -5496,7 +5765,7 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5521,30 +5790,30 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -5556,7 +5825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5572,7 +5841,7 @@
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -5597,17 +5866,17 @@
         <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -5621,17 +5890,17 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -5643,7 +5912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A3:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5664,13 +5933,13 @@
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -5679,10 +5948,10 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
         <v>120</v>
-      </c>
-      <c r="H3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5690,10 +5959,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -5705,22 +5974,22 @@
         <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5728,10 +5997,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
@@ -5745,17 +6014,17 @@
         <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5763,10 +6032,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
@@ -5778,17 +6047,17 @@
         <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5796,10 +6065,10 @@
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
@@ -5813,17 +6082,17 @@
         <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -5835,10 +6104,10 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5846,17 +6115,17 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5870,10 +6139,10 @@
         <v>14</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5881,17 +6150,17 @@
         <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -5903,10 +6172,10 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -5914,17 +6183,17 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -5938,10 +6207,10 @@
         <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -5949,17 +6218,17 @@
         <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -5971,28 +6240,28 @@
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -6004,7 +6273,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A3:N44"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
@@ -6030,7 +6299,7 @@
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
@@ -6042,13 +6311,13 @@
         <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I3" t="s">
         <v>41</v>
@@ -6060,13 +6329,13 @@
         <v>11</v>
       </c>
       <c r="L3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3" t="s">
         <v>120</v>
       </c>
-      <c r="M3" t="s">
-        <v>121</v>
-      </c>
       <c r="N3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6102,10 +6371,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -6122,7 +6391,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -6139,7 +6408,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -6156,7 +6425,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -6173,7 +6442,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -6221,10 +6490,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -6241,7 +6510,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -6258,7 +6527,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -6275,7 +6544,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -6292,7 +6561,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -6335,10 +6604,10 @@
         <v>10</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="N16" s="1"/>
     </row>
@@ -6347,7 +6616,7 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -6364,7 +6633,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -6381,7 +6650,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -6398,7 +6667,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -6425,11 +6694,11 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>38</v>
@@ -6449,7 +6718,7 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -6466,7 +6735,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -6483,7 +6752,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -6500,7 +6769,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -6527,11 +6796,11 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>38</v>
@@ -6551,7 +6820,7 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -6568,7 +6837,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -6585,7 +6854,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -6602,7 +6871,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -6629,11 +6898,11 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>38</v>
@@ -6645,10 +6914,10 @@
         <v>10</v>
       </c>
       <c r="L31" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M31" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="N31" s="1"/>
     </row>
@@ -6657,7 +6926,7 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -6674,7 +6943,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -6691,7 +6960,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -6708,7 +6977,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -6735,11 +7004,11 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>38</v>
@@ -6751,10 +7020,10 @@
         <v>10</v>
       </c>
       <c r="L36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M36" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="N36" s="1"/>
     </row>
@@ -6763,7 +7032,7 @@
         <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -6780,7 +7049,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -6797,7 +7066,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -6814,7 +7083,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -6841,7 +7110,7 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>37</v>
@@ -6859,7 +7128,7 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -6867,7 +7136,7 @@
         <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -6884,7 +7153,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -6901,7 +7170,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>

</xml_diff>

<commit_message>
begun final pattern selection
</commit_message>
<xml_diff>
--- a/readkeyboard_options.xlsx
+++ b/readkeyboard_options.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeffKarle\Documents\cinder_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EECBEC-A331-4D5A-A5A8-3AFEAFB64A3F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5475" windowWidth="18375" windowHeight="9675" tabRatio="765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13005" windowHeight="5505" tabRatio="765" firstSheet="12" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="keyboard" sheetId="1" r:id="rId1"/>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="217">
   <si>
     <t>letter</t>
   </si>
@@ -693,12 +692,15 @@
   </si>
   <si>
     <t>get variables</t>
+  </si>
+  <si>
+    <t>brightness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -906,7 +908,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="64">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1110,334 +1115,335 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B4:E30" totalsRowShown="0">
-  <autoFilter ref="B4:E30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:E30" totalsRowShown="0">
+  <autoFilter ref="B4:E30"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ascii "/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="letter"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="variable"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="range"/>
+    <tableColumn id="1" name="ascii "/>
+    <tableColumn id="2" name="letter"/>
+    <tableColumn id="3" name="variable"/>
+    <tableColumn id="4" name="range"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table16" displayName="Table16" ref="C4:I18" totalsRowShown="0">
-  <autoFilter ref="C4:I18" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="C4:I18" totalsRowShown="0">
+  <autoFilter ref="C4:I18"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="this_rot" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="this_delay" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="target_palette" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="bg_clr" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="bg_bri" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="this_fade" dataDxfId="45"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_rot" dataDxfId="51"/>
+    <tableColumn id="3" name="this_delay" dataDxfId="50"/>
+    <tableColumn id="4" name="target_palette" dataDxfId="49"/>
+    <tableColumn id="5" name="bg_clr" dataDxfId="48"/>
+    <tableColumn id="6" name="bg_bri" dataDxfId="47"/>
+    <tableColumn id="7" name="this_fade" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table21" displayName="Table21" ref="B5:M11" totalsRowShown="0">
-  <autoFilter ref="B5:M11" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="B5:M11" totalsRowShown="0">
+  <autoFilter ref="B5:M11"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="this_fade" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="this_delay" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="blue_angle" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="blue_low" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="blue_high" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="green_angle" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="green_low" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="green_high" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="red_angle" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="red_low" dataDxfId="35"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="red_high" dataDxfId="34"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_fade" dataDxfId="45"/>
+    <tableColumn id="3" name="this_delay" dataDxfId="44"/>
+    <tableColumn id="4" name="blue_angle" dataDxfId="43"/>
+    <tableColumn id="5" name="blue_low" dataDxfId="42"/>
+    <tableColumn id="6" name="blue_high" dataDxfId="41"/>
+    <tableColumn id="7" name="green_angle" dataDxfId="40"/>
+    <tableColumn id="8" name="green_low" dataDxfId="39"/>
+    <tableColumn id="9" name="green_high" dataDxfId="38"/>
+    <tableColumn id="10" name="red_angle" dataDxfId="37"/>
+    <tableColumn id="11" name="red_low" dataDxfId="36"/>
+    <tableColumn id="12" name="red_high" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table9" displayName="Table9" ref="B3:H20" totalsRowShown="0">
-  <autoFilter ref="B3:H20" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="B3:H20" totalsRowShown="0">
+  <autoFilter ref="B3:H20"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="scale" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="scale2" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="this_delay" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="target_palette" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="Column1" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="b" dataDxfId="28"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="scale" dataDxfId="34"/>
+    <tableColumn id="5" name="scale2" dataDxfId="33"/>
+    <tableColumn id="3" name="this_delay" dataDxfId="32"/>
+    <tableColumn id="4" name="target_palette" dataDxfId="31"/>
+    <tableColumn id="6" name="Column1" dataDxfId="30"/>
+    <tableColumn id="7" name="b" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table10" displayName="Table10" ref="C4:L14" totalsRowShown="0">
-  <autoFilter ref="C4:L14" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="C4:L14" totalsRowShown="0">
+  <autoFilter ref="C4:L14"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="this_inc"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="this_speed"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="all_freq"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="this_cutoff"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="bg_clr"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="bg_bri"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="this_rot"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="this_delay"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="target_palette"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_inc"/>
+    <tableColumn id="3" name="this_speed"/>
+    <tableColumn id="4" name="all_freq"/>
+    <tableColumn id="5" name="this_cutoff"/>
+    <tableColumn id="6" name="bg_clr"/>
+    <tableColumn id="7" name="bg_bri"/>
+    <tableColumn id="8" name="this_rot"/>
+    <tableColumn id="9" name="this_delay"/>
+    <tableColumn id="10" name="target_palette"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table11" displayName="Table11" ref="C4:E9" totalsRowShown="0">
-  <autoFilter ref="C4:E9" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="C4:E9" totalsRowShown="0">
+  <autoFilter ref="C4:E9"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="this_delay"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="target_palette"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_delay"/>
+    <tableColumn id="3" name="target_palette"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="C4:F16" totalsRowShown="0">
-  <autoFilter ref="C4:F16" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="C4:F16" totalsRowShown="0">
+  <autoFilter ref="C4:F16"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="this_rot"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="this_diff"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="this_delay"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_rot"/>
+    <tableColumn id="3" name="this_diff"/>
+    <tableColumn id="4" name="this_delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table2" displayName="Table2" ref="C4:G10" totalsRowShown="0">
-  <autoFilter ref="C4:G10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C4:G10" totalsRowShown="0">
+  <autoFilter ref="C4:G10"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="this_fade"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="this_delay"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="target_palette"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="myfade"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_fade"/>
+    <tableColumn id="3" name="this_delay"/>
+    <tableColumn id="4" name="target_palette"/>
+    <tableColumn id="5" name="myfade"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table13" displayName="Table13" ref="C4:F14" totalsRowShown="0">
-  <autoFilter ref="C4:F14" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="C4:F14" totalsRowShown="0">
+  <autoFilter ref="C4:F14"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="this_delay"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="target_palette"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="this_fade"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_delay"/>
+    <tableColumn id="3" name="target_palette"/>
+    <tableColumn id="4" name="this_fade"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table14" displayName="Table14" ref="C5:P44" totalsRowShown="0">
-  <autoFilter ref="C5:P44" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="C5:P44" totalsRowShown="0">
+  <autoFilter ref="C5:P44"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="mode"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="spiral_width" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="spiral_inc" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="this_hue" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="this_inc" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1100-000009000000}" name="this_speed" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1100-00000A000000}" name="this_rot" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1100-00000B000000}" name="all_freq" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{224737A4-F2E0-4741-A037-78BAF37DC825}" name="this_cutoff" dataDxfId="0"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1100-00000E000000}" name="that_speed" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1100-00000C000000}" name="bg_clr" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1100-00000D000000}" name="bg_bri" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="this_delay" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="target_palette" dataDxfId="16"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="3" name="spiral_width" dataDxfId="28"/>
+    <tableColumn id="6" name="spiral_inc" dataDxfId="27"/>
+    <tableColumn id="4" name="this_hue" dataDxfId="26"/>
+    <tableColumn id="8" name="this_inc" dataDxfId="25"/>
+    <tableColumn id="9" name="this_speed" dataDxfId="24"/>
+    <tableColumn id="10" name="this_rot" dataDxfId="23"/>
+    <tableColumn id="11" name="all_freq" dataDxfId="22"/>
+    <tableColumn id="2" name="this_cutoff" dataDxfId="21"/>
+    <tableColumn id="14" name="that_speed" dataDxfId="20"/>
+    <tableColumn id="12" name="bg_clr" dataDxfId="19"/>
+    <tableColumn id="13" name="bg_bri" dataDxfId="18"/>
+    <tableColumn id="5" name="this_delay" dataDxfId="17"/>
+    <tableColumn id="7" name="target_palette" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table19" displayName="Table19" ref="C3:J6" totalsRowShown="0">
-  <autoFilter ref="C3:J6" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="C3:J6" totalsRowShown="0">
+  <autoFilter ref="C3:J6"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="twinkle_speed"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="twinkle_density"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="twinkle_bg"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="auto_select_background_color"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="cool_like_incandescent"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1200-000008000000}" name="this_delay"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1200-000009000000}" name="target_palette"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="twinkle_speed"/>
+    <tableColumn id="3" name="twinkle_density"/>
+    <tableColumn id="4" name="twinkle_bg"/>
+    <tableColumn id="5" name="auto_select_background_color"/>
+    <tableColumn id="7" name="cool_like_incandescent"/>
+    <tableColumn id="8" name="this_delay"/>
+    <tableColumn id="9" name="target_palette"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="B3:G15" totalsRowShown="0">
-  <autoFilter ref="B3:G15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:G15" totalsRowShown="0">
+  <autoFilter ref="B3:G15"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="this_fade"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="vImpact0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="target_palette"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="this_delay"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Column1"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_fade"/>
+    <tableColumn id="3" name="vImpact0"/>
+    <tableColumn id="4" name="target_palette"/>
+    <tableColumn id="5" name="this_delay"/>
+    <tableColumn id="6" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table15" displayName="Table15" ref="C5:H13" totalsRowShown="0">
-  <autoFilter ref="C5:H13" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="C5:H15" totalsRowShown="0">
+  <autoFilter ref="C5:H15"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="mul1" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="mul2" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="mul3" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="this_delay" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1300-000006000000}" name="target_palette" dataDxfId="11"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="mul1" dataDxfId="15"/>
+    <tableColumn id="3" name="mul2" dataDxfId="14"/>
+    <tableColumn id="4" name="mul3" dataDxfId="13"/>
+    <tableColumn id="5" name="this_delay" dataDxfId="12"/>
+    <tableColumn id="6" name="target_palette" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Table17" displayName="Table17" ref="C4:M19" totalsRowShown="0">
-  <autoFilter ref="C4:M19" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="this_speed" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="that_speed" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="this_rot" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1400-000005000000}" name="that_rot" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1400-000006000000}" name="all_freq" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1400-000008000000}" name="this_cutoff" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1400-000009000000}" name="that_cutoff" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1400-00000A000000}" name="this_sat" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1400-00000B000000}" name="this_delay" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1400-00000C000000}" name="target_palette" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="C4:N19" totalsRowShown="0">
+  <autoFilter ref="C4:N19"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_speed" dataDxfId="10"/>
+    <tableColumn id="3" name="that_speed" dataDxfId="9"/>
+    <tableColumn id="4" name="this_rot" dataDxfId="8"/>
+    <tableColumn id="5" name="that_rot" dataDxfId="7"/>
+    <tableColumn id="6" name="all_freq" dataDxfId="6"/>
+    <tableColumn id="8" name="this_cutoff" dataDxfId="5"/>
+    <tableColumn id="9" name="that_cutoff" dataDxfId="4"/>
+    <tableColumn id="10" name="this_sat" dataDxfId="3"/>
+    <tableColumn id="11" name="this_delay" dataDxfId="2"/>
+    <tableColumn id="12" name="target_palette" dataDxfId="1"/>
+    <tableColumn id="7" name="brightness" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="B4:F24" totalsRowShown="0">
-  <autoFilter ref="B4:F24" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B4:F24" totalsRowShown="0">
+  <autoFilter ref="B4:F24"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="scale"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="target_palette"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="this_delay"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Notes"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="scale"/>
+    <tableColumn id="3" name="target_palette"/>
+    <tableColumn id="5" name="this_delay"/>
+    <tableColumn id="4" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="B3:D10" totalsRowShown="0">
-  <autoFilter ref="B3:D10" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B3:D10" totalsRowShown="0">
+  <autoFilter ref="B3:D10"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="target_palette"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="this_delay"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="target_palette"/>
+    <tableColumn id="3" name="this_delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table20" displayName="Table20" ref="B4:E8" totalsRowShown="0">
-  <autoFilter ref="B4:E8" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="B4:E8" totalsRowShown="0">
+  <autoFilter ref="B4:E8"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="this_delay "/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="target_palette"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Column1"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_delay "/>
+    <tableColumn id="3" name="target_palette"/>
+    <tableColumn id="4" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="B3:H9" totalsRowShown="0">
-  <autoFilter ref="B3:H9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B3:H9" totalsRowShown="0">
+  <autoFilter ref="B3:H9"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="this_diff"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="this_inc"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="this_fade"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="target_palette"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="this_delay"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Notes"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_diff"/>
+    <tableColumn id="3" name="this_inc"/>
+    <tableColumn id="7" name="this_fade"/>
+    <tableColumn id="4" name="target_palette"/>
+    <tableColumn id="5" name="this_delay"/>
+    <tableColumn id="6" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table18" displayName="Table18" ref="C4:G12" totalsRowShown="0">
-  <autoFilter ref="C4:G12" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="C4:G12" totalsRowShown="0">
+  <autoFilter ref="C4:G12"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="this_hue"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="this_inc"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="this_delay"/>
-    <tableColumn id="5" xr3:uid="{3CD86568-346E-42F4-8A83-60AE3B2E2A56}" name="Column1"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_hue"/>
+    <tableColumn id="4" name="this_inc"/>
+    <tableColumn id="3" name="this_delay"/>
+    <tableColumn id="5" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table8" displayName="Table8" ref="B3:H40" totalsRowShown="0">
-  <autoFilter ref="B3:H40" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:H40" totalsRowShown="0">
+  <autoFilter ref="B3:H40"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="cooling"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="sparking"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="this_delay"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="target_palette"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="cooling1-4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="sparking1-4"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="cooling"/>
+    <tableColumn id="3" name="sparking"/>
+    <tableColumn id="4" name="this_delay"/>
+    <tableColumn id="5" name="target_palette"/>
+    <tableColumn id="6" name="cooling1-4"/>
+    <tableColumn id="7" name="sparking1-4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table7" displayName="Table7" ref="B3:N44" totalsRowShown="0">
-  <autoFilter ref="B3:N44" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:N44" totalsRowShown="0">
+  <autoFilter ref="B3:N44"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="juggle_index_reset" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="this_fade" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="numdots_ring" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="numdots" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="this_beat" dataDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="ringBeat" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="this_diff" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="target_palette" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="this_delay" dataDxfId="54"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="cooling1-4" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="sparking1-4" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="jug16_phase" dataDxfId="51"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="juggle_index_reset" dataDxfId="63"/>
+    <tableColumn id="3" name="this_fade" dataDxfId="62"/>
+    <tableColumn id="4" name="numdots_ring" dataDxfId="61"/>
+    <tableColumn id="12" name="numdots" dataDxfId="60"/>
+    <tableColumn id="5" name="this_beat" dataDxfId="59"/>
+    <tableColumn id="13" name="ringBeat" dataDxfId="58"/>
+    <tableColumn id="6" name="this_diff" dataDxfId="57"/>
+    <tableColumn id="7" name="target_palette" dataDxfId="56"/>
+    <tableColumn id="8" name="this_delay" dataDxfId="55"/>
+    <tableColumn id="11" name="cooling1-4" dataDxfId="54"/>
+    <tableColumn id="10" name="sparking1-4" dataDxfId="53"/>
+    <tableColumn id="9" name="jug16_phase" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1739,13 +1745,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B4:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -2415,7 +2421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I18"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
@@ -2666,7 +2672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2842,7 +2848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
@@ -3155,11 +3161,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3257,11 +3263,20 @@
       <c r="G6">
         <v>180</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
       <c r="J6">
         <v>8</v>
       </c>
       <c r="K6">
         <v>4</v>
+      </c>
+      <c r="L6">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -3318,10 +3333,64 @@
       <c r="C11" t="s">
         <v>134</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>180</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>134</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>224</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -3343,7 +3412,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3410,7 +3479,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3538,7 +3607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3624,11 +3693,11 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3674,6 +3743,15 @@
       <c r="C6" t="s">
         <v>138</v>
       </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -3694,6 +3772,15 @@
       <c r="C10" s="1">
         <v>34</v>
       </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -3701,6 +3788,15 @@
       </c>
       <c r="C11" t="s">
         <v>139</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -3727,7 +3823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:Q44"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4637,7 +4733,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4714,7 +4810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4902,11 +4998,11 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="B5:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4963,20 +5059,38 @@
       <c r="C7" t="s">
         <v>158</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>15</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -5016,31 +5130,88 @@
       <c r="C11" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="D12" s="1">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>18</v>
+      </c>
+      <c r="H12" s="1">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>159</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5052,11 +5223,11 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="B4:M19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5075,7 +5246,7 @@
     <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>57</v>
       </c>
@@ -5109,8 +5280,11 @@
       <c r="M4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>48</v>
       </c>
@@ -5142,71 +5316,156 @@
         <v>10</v>
       </c>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>18</v>
+      </c>
+      <c r="I6" s="1">
+        <v>128</v>
+      </c>
+      <c r="J6" s="1">
+        <v>160</v>
+      </c>
+      <c r="K6" s="1">
+        <v>255</v>
+      </c>
+      <c r="L6" s="1">
+        <v>10</v>
+      </c>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>253</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1">
+        <v>128</v>
+      </c>
+      <c r="J7" s="1">
+        <v>128</v>
+      </c>
+      <c r="K7" s="1">
+        <v>255</v>
+      </c>
+      <c r="L7" s="1">
+        <v>12</v>
+      </c>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1">
+        <v>128</v>
+      </c>
+      <c r="J8" s="1">
+        <v>32</v>
+      </c>
+      <c r="K8" s="1">
+        <v>255</v>
+      </c>
+      <c r="L8" s="1">
+        <v>10</v>
+      </c>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>160</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>255</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1">
+        <v>64</v>
+      </c>
+      <c r="J9" s="1">
+        <v>128</v>
+      </c>
+      <c r="K9" s="1">
+        <v>255</v>
+      </c>
+      <c r="L9" s="1">
+        <v>10</v>
+      </c>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <v>49</v>
       </c>
@@ -5238,41 +5497,82 @@
         <v>10</v>
       </c>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>163</v>
       </c>
       <c r="C11" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>253</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1">
+        <v>128</v>
+      </c>
+      <c r="J11" s="1">
+        <v>64</v>
+      </c>
+      <c r="K11" s="1">
+        <v>255</v>
+      </c>
+      <c r="L11" s="1">
+        <v>10</v>
+      </c>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="D12" s="1">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>255</v>
+      </c>
+      <c r="L12" s="1">
+        <v>10</v>
+      </c>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>161</v>
       </c>
@@ -5286,8 +5586,9 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>161</v>
       </c>
@@ -5301,8 +5602,9 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>50</v>
       </c>
@@ -5327,33 +5629,59 @@
       <c r="J15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="L15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>52</v>
       </c>
       <c r="C16" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>253</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1">
+        <v>64</v>
+      </c>
+      <c r="J16" s="1">
+        <v>128</v>
+      </c>
+      <c r="K16" s="1">
+        <v>255</v>
+      </c>
+      <c r="L16" s="1">
+        <v>15</v>
+      </c>
+      <c r="M16" s="1">
+        <v>66</v>
+      </c>
+      <c r="N16" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>162</v>
       </c>
@@ -5367,8 +5695,9 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>162</v>
       </c>
@@ -5382,8 +5711,9 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>162</v>
       </c>
@@ -5397,6 +5727,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5407,7 +5738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
@@ -5599,7 +5930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5677,7 +6008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5745,7 +6076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5842,7 +6173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5949,7 +6280,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H40"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
@@ -6310,7 +6641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N44"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="77" workbookViewId="0">

</xml_diff>

<commit_message>
final script updates with serial
</commit_message>
<xml_diff>
--- a/readkeyboard_options.xlsx
+++ b/readkeyboard_options.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeffKarle\Documents\cinder_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4FF310-3A00-457C-91BE-F1FA9B98F5A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22395" yWindow="3765" windowWidth="21810" windowHeight="12525" tabRatio="765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22395" yWindow="3765" windowWidth="21810" windowHeight="12525" tabRatio="765"/>
   </bookViews>
   <sheets>
     <sheet name="keyboard" sheetId="1" r:id="rId1"/>
@@ -36,7 +35,7 @@
     <sheet name="three_sin" sheetId="15" r:id="rId21"/>
     <sheet name="two_sin" sheetId="16" r:id="rId22"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="254">
   <si>
     <t>letter</t>
   </si>
@@ -567,9 +566,6 @@
     <t>jug16_phase</t>
   </si>
   <si>
-    <t>d10</t>
-  </si>
-  <si>
     <t>omg</t>
   </si>
   <si>
@@ -606,12 +602,6 @@
     <t>red_high</t>
   </si>
   <si>
-    <t>d5</t>
-  </si>
-  <si>
-    <t>d1</t>
-  </si>
-  <si>
     <t>change to this_inc</t>
   </si>
   <si>
@@ -817,12 +807,18 @@
   </si>
   <si>
     <t>rand(palette)</t>
+  </si>
+  <si>
+    <t>make mode 61 and 62 happen at the same time</t>
+  </si>
+  <si>
+    <t>slowly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1038,50 +1034,88 @@
   </cellStyles>
   <dxfs count="77">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1235,88 +1269,50 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1332,370 +1328,371 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B4:E30" totalsRowShown="0">
-  <autoFilter ref="B4:E30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:E30" totalsRowShown="0">
+  <autoFilter ref="B4:E30"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ascii "/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="letter"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="variable"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="range"/>
+    <tableColumn id="1" name="ascii "/>
+    <tableColumn id="2" name="letter"/>
+    <tableColumn id="3" name="variable"/>
+    <tableColumn id="4" name="range"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table8" displayName="Table8" ref="B3:I38" totalsRowShown="0">
-  <autoFilter ref="B3:I38" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:I38" totalsRowShown="0">
+  <autoFilter ref="B3:I38"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="cooling" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="sparking" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="this_delay" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="target_palette" dataDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="cooling1-4" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="sparking1-4" dataDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="sparking1-5" dataDxfId="70"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="cooling" dataDxfId="74"/>
+    <tableColumn id="3" name="sparking" dataDxfId="73"/>
+    <tableColumn id="4" name="this_delay" dataDxfId="72"/>
+    <tableColumn id="5" name="target_palette" dataDxfId="71"/>
+    <tableColumn id="6" name="cooling1-4" dataDxfId="70"/>
+    <tableColumn id="7" name="sparking1-4" dataDxfId="69"/>
+    <tableColumn id="8" name="sparking1-5" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table23" displayName="Table23" ref="C3:H8" totalsRowShown="0">
-  <autoFilter ref="C3:H8" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table23" displayName="Table23" ref="C3:H8" totalsRowShown="0">
+  <autoFilter ref="C3:H8"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="this_fade"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="this_delay"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="streamer_velocity"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="explosion_velocity"/>
-    <tableColumn id="6" xr3:uid="{33A2169D-5FC7-454A-BBF4-A3D0C439B678}" name="Column1"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_fade"/>
+    <tableColumn id="3" name="this_delay"/>
+    <tableColumn id="4" name="streamer_velocity"/>
+    <tableColumn id="5" name="explosion_velocity"/>
+    <tableColumn id="6" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table7" displayName="Table7" ref="B3:N41" totalsRowShown="0">
-  <autoFilter ref="B3:N41" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:N41" totalsRowShown="0">
+  <autoFilter ref="B3:N41"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="mode"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="this_delay" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="target_palette" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="juggle_index_reset" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="this_fade" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="numdots_ring" dataDxfId="67"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="numdots_ring_arr[]" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="this_beat" dataDxfId="65"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0A00-00000D000000}" name="ringBeat" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="this_diff" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="cooling1-4" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="sparking1-4" dataDxfId="61"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="jug16_phase" dataDxfId="60"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="8" name="this_delay" dataDxfId="67"/>
+    <tableColumn id="7" name="target_palette" dataDxfId="66"/>
+    <tableColumn id="2" name="juggle_index_reset" dataDxfId="65"/>
+    <tableColumn id="3" name="this_fade" dataDxfId="64"/>
+    <tableColumn id="4" name="numdots_ring" dataDxfId="63"/>
+    <tableColumn id="12" name="numdots_ring_arr[]" dataDxfId="62"/>
+    <tableColumn id="5" name="this_beat" dataDxfId="61"/>
+    <tableColumn id="13" name="ringBeat" dataDxfId="60"/>
+    <tableColumn id="6" name="this_diff" dataDxfId="59"/>
+    <tableColumn id="11" name="cooling1-4" dataDxfId="58"/>
+    <tableColumn id="10" name="sparking1-4" dataDxfId="57"/>
+    <tableColumn id="9" name="jug16_phase" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="C4:K18" totalsRowShown="0">
-  <autoFilter ref="C4:K18" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="C4:K18" totalsRowShown="0">
+  <autoFilter ref="C4:K18"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="this_rot" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="this_delay" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="target_palette" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="bg_clr" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="bg_bri" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="this_fade" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="Column1" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0B00-000009000000}" name="Column2" dataDxfId="52"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_rot" dataDxfId="55"/>
+    <tableColumn id="3" name="this_delay" dataDxfId="54"/>
+    <tableColumn id="4" name="target_palette" dataDxfId="53"/>
+    <tableColumn id="5" name="bg_clr" dataDxfId="52"/>
+    <tableColumn id="6" name="bg_bri" dataDxfId="51"/>
+    <tableColumn id="7" name="this_fade" dataDxfId="50"/>
+    <tableColumn id="8" name="Column1" dataDxfId="49"/>
+    <tableColumn id="9" name="Column2" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table21" displayName="Table21" ref="B5:M11" totalsRowShown="0">
-  <autoFilter ref="B5:M11" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="B5:M11" totalsRowShown="0">
+  <autoFilter ref="B5:M11"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="this_fade" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="this_delay" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="blue_angle" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="blue_low" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="blue_high" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="green_angle" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="green_low" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="green_high" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="red_angle" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0C00-00000B000000}" name="red_low" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0C00-00000C000000}" name="red_high" dataDxfId="41"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_fade" dataDxfId="47"/>
+    <tableColumn id="3" name="this_delay" dataDxfId="46"/>
+    <tableColumn id="4" name="blue_angle" dataDxfId="45"/>
+    <tableColumn id="5" name="blue_low" dataDxfId="44"/>
+    <tableColumn id="6" name="blue_high" dataDxfId="43"/>
+    <tableColumn id="7" name="green_angle" dataDxfId="42"/>
+    <tableColumn id="8" name="green_low" dataDxfId="41"/>
+    <tableColumn id="9" name="green_high" dataDxfId="40"/>
+    <tableColumn id="10" name="red_angle" dataDxfId="39"/>
+    <tableColumn id="11" name="red_low" dataDxfId="38"/>
+    <tableColumn id="12" name="red_high" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table9" displayName="Table9" ref="B3:I20" totalsRowShown="0">
-  <autoFilter ref="B3:I20" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="B3:I20" totalsRowShown="0">
+  <autoFilter ref="B3:I20"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="scale" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="scale2" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="this_delay" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="target_palette" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="Column1" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="b" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="Column2" dataDxfId="34"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="scale" dataDxfId="36"/>
+    <tableColumn id="5" name="scale2" dataDxfId="35"/>
+    <tableColumn id="3" name="this_delay" dataDxfId="34"/>
+    <tableColumn id="4" name="target_palette" dataDxfId="33"/>
+    <tableColumn id="6" name="Column1" dataDxfId="32"/>
+    <tableColumn id="7" name="b" dataDxfId="31"/>
+    <tableColumn id="8" name="Column2" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table10" displayName="Table10" ref="C4:L14" totalsRowShown="0">
-  <autoFilter ref="C4:L14" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="C4:L14" totalsRowShown="0">
+  <autoFilter ref="C4:L14"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="this_inc"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="this_speed"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="all_freq"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="this_cutoff"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="bg_clr"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" name="bg_bri"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="this_rot"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="this_delay"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0E00-00000A000000}" name="target_palette"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_inc"/>
+    <tableColumn id="3" name="this_speed"/>
+    <tableColumn id="4" name="all_freq"/>
+    <tableColumn id="5" name="this_cutoff"/>
+    <tableColumn id="6" name="bg_clr"/>
+    <tableColumn id="7" name="bg_bri"/>
+    <tableColumn id="8" name="this_rot"/>
+    <tableColumn id="9" name="this_delay"/>
+    <tableColumn id="10" name="target_palette"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="C4:E9" totalsRowShown="0">
-  <autoFilter ref="C4:E9" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="C4:E9" totalsRowShown="0">
+  <autoFilter ref="C4:E9"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="this_delay"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="target_palette"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_delay"/>
+    <tableColumn id="3" name="target_palette"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table12" displayName="Table12" ref="C4:F16" totalsRowShown="0">
-  <autoFilter ref="C4:F16" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="C4:F16" totalsRowShown="0">
+  <autoFilter ref="C4:F16"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="this_rot"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="this_diff"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="this_delay"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_rot"/>
+    <tableColumn id="3" name="this_diff"/>
+    <tableColumn id="4" name="this_delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table2" displayName="Table2" ref="C4:G10" totalsRowShown="0">
-  <autoFilter ref="C4:G10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C4:G10" totalsRowShown="0">
+  <autoFilter ref="C4:G10"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="this_fade"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="this_delay"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="target_palette"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="myfade"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_fade"/>
+    <tableColumn id="3" name="this_delay"/>
+    <tableColumn id="4" name="target_palette"/>
+    <tableColumn id="5" name="myfade"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{2CB0AF64-2043-4AFC-9DD2-7851A54AF5A8}" name="Table24" displayName="Table24" ref="O12:Q16" totalsRowShown="0">
-  <autoFilter ref="O12:Q16" xr:uid="{FBE668EB-B6DB-4D5A-832E-ECE4A1789878}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{105CB44F-EEA5-4D26-B564-88DF596DC969}" name="Rotary Function"/>
-    <tableColumn id="4" xr3:uid="{0335C800-CF48-4B73-8912-9D69E644716D}" name="Rotate"/>
-    <tableColumn id="2" xr3:uid="{5152827C-77A3-45CE-B6C2-349AD70B9611}" name="SwitchB On"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="O12:R18" totalsRowShown="0">
+  <autoFilter ref="O12:R18"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Rotary Function"/>
+    <tableColumn id="4" name="Rotate"/>
+    <tableColumn id="2" name="SwitchB On"/>
+    <tableColumn id="3" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table13" displayName="Table13" ref="C4:F14" totalsRowShown="0">
-  <autoFilter ref="C4:F14" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="C4:F14" totalsRowShown="0">
+  <autoFilter ref="C4:F14"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="this_delay"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="target_palette"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="this_fade"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_delay"/>
+    <tableColumn id="3" name="target_palette"/>
+    <tableColumn id="4" name="this_fade"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table14" displayName="Table14" ref="C5:O22" totalsRowShown="0">
-  <autoFilter ref="C5:O22" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="C5:O22" totalsRowShown="0">
+  <autoFilter ref="C5:O22"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="mode"/>
-    <tableColumn id="3" xr3:uid="{6905E999-B173-4864-BB8A-BC6D37BB6ABC}" name="d" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{A76E4A82-7488-48AF-B7BE-76BD0688E035}" name="f " dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1300-000008000000}" name="this_inc" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1300-000009000000}" name="this_speed" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1300-00000A000000}" name="this_rot" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1300-00000B000000}" name="all_freq" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="this_cutoff" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1300-00000E000000}" name="that_speed" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1300-00000C000000}" name="bg_clr" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1300-00000D000000}" name="bg_bri" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="this_delay" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1300-000007000000}" name="target_palette" dataDxfId="24"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="3" name="d" dataDxfId="29"/>
+    <tableColumn id="4" name="f " dataDxfId="28"/>
+    <tableColumn id="8" name="this_inc" dataDxfId="27"/>
+    <tableColumn id="9" name="this_speed" dataDxfId="26"/>
+    <tableColumn id="10" name="this_rot" dataDxfId="25"/>
+    <tableColumn id="11" name="all_freq" dataDxfId="24"/>
+    <tableColumn id="2" name="this_cutoff" dataDxfId="23"/>
+    <tableColumn id="14" name="that_speed" dataDxfId="22"/>
+    <tableColumn id="12" name="bg_clr" dataDxfId="21"/>
+    <tableColumn id="13" name="bg_bri" dataDxfId="20"/>
+    <tableColumn id="5" name="this_delay" dataDxfId="19"/>
+    <tableColumn id="7" name="target_palette" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Table19" displayName="Table19" ref="C3:E6" totalsRowShown="0">
-  <autoFilter ref="C3:E6" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="C3:E6" totalsRowShown="0">
+  <autoFilter ref="C3:E6"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="mode"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1400-000008000000}" name="this_delay" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1400-000009000000}" name="target_palette" dataDxfId="22"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="8" name="this_delay" dataDxfId="17"/>
+    <tableColumn id="9" name="target_palette" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Table15" displayName="Table15" ref="C5:H15" totalsRowShown="0">
-  <autoFilter ref="C5:H15" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="C5:H15" totalsRowShown="0">
+  <autoFilter ref="C5:H15"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="mul1" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" name="mul2" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="mul3" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" name="this_delay" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1500-000006000000}" name="target_palette" dataDxfId="17"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="mul1" dataDxfId="15"/>
+    <tableColumn id="3" name="mul2" dataDxfId="14"/>
+    <tableColumn id="4" name="mul3" dataDxfId="13"/>
+    <tableColumn id="5" name="this_delay" dataDxfId="12"/>
+    <tableColumn id="6" name="target_palette" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="Table17" displayName="Table17" ref="C4:N19" totalsRowShown="0">
-  <autoFilter ref="C4:N19" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="C4:N19" totalsRowShown="0">
+  <autoFilter ref="C4:N19"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="this_speed" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1600-000003000000}" name="that_speed" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="this_rot" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1600-000005000000}" name="that_rot" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1600-000006000000}" name="all_freq" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1600-000008000000}" name="this_cutoff" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1600-000009000000}" name="that_cutoff" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1600-00000A000000}" name="this_sat" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1600-00000B000000}" name="this_delay" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1600-00000C000000}" name="target_palette" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1600-000007000000}" name="brightness" dataDxfId="6"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_speed" dataDxfId="10"/>
+    <tableColumn id="3" name="that_speed" dataDxfId="9"/>
+    <tableColumn id="4" name="this_rot" dataDxfId="8"/>
+    <tableColumn id="5" name="that_rot" dataDxfId="7"/>
+    <tableColumn id="6" name="all_freq" dataDxfId="6"/>
+    <tableColumn id="8" name="this_cutoff" dataDxfId="5"/>
+    <tableColumn id="9" name="that_cutoff" dataDxfId="4"/>
+    <tableColumn id="10" name="this_sat" dataDxfId="3"/>
+    <tableColumn id="11" name="this_delay" dataDxfId="2"/>
+    <tableColumn id="12" name="target_palette" dataDxfId="1"/>
+    <tableColumn id="7" name="brightness" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table22" displayName="Table22" ref="L4:M97" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="L4:M97" xr:uid="{00000000-0009-0000-0100-000016000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="L4:M97" totalsRowShown="0" headerRowDxfId="76">
+  <autoFilter ref="L4:M97"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="led_mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="mode" dataDxfId="0"/>
+    <tableColumn id="1" name="led_mode"/>
+    <tableColumn id="2" name="mode" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:F15" totalsRowShown="0">
-  <autoFilter ref="B3:F15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:F15" totalsRowShown="0">
+  <autoFilter ref="B3:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="this_fade"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="target_palette"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="this_delay"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Column1"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_fade"/>
+    <tableColumn id="4" name="target_palette"/>
+    <tableColumn id="5" name="this_delay"/>
+    <tableColumn id="6" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="B4:F24" totalsRowShown="0">
-  <autoFilter ref="B4:F24" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B4:F24" totalsRowShown="0">
+  <autoFilter ref="B4:F24"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="scale"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="target_palette"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="this_delay"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Notes"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="scale"/>
+    <tableColumn id="3" name="target_palette"/>
+    <tableColumn id="5" name="this_delay"/>
+    <tableColumn id="4" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table5" displayName="Table5" ref="B3:D10" totalsRowShown="0">
-  <autoFilter ref="B3:D10" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B3:D10" totalsRowShown="0">
+  <autoFilter ref="B3:D10"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="target_palette"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="this_delay"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="target_palette"/>
+    <tableColumn id="3" name="this_delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table20" displayName="Table20" ref="B4:E8" totalsRowShown="0">
-  <autoFilter ref="B4:E8" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="B4:E8" totalsRowShown="0">
+  <autoFilter ref="B4:E8"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="this_delay "/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="target_palette"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Column1"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_delay "/>
+    <tableColumn id="3" name="target_palette"/>
+    <tableColumn id="4" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table6" displayName="Table6" ref="B3:H9" totalsRowShown="0">
-  <autoFilter ref="B3:H9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B3:H9" totalsRowShown="0">
+  <autoFilter ref="B3:H9"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="this_diff"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="this_inc"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="this_fade"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="target_palette"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="this_delay"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Notes"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_diff"/>
+    <tableColumn id="3" name="this_inc"/>
+    <tableColumn id="7" name="this_fade"/>
+    <tableColumn id="4" name="target_palette"/>
+    <tableColumn id="5" name="this_delay"/>
+    <tableColumn id="6" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table18" displayName="Table18" ref="C4:G12" totalsRowShown="0">
-  <autoFilter ref="C4:G12" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="C4:G12" totalsRowShown="0">
+  <autoFilter ref="C4:G12"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="mode"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="this_hue"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="this_inc"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="this_delay"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Column1"/>
+    <tableColumn id="1" name="mode"/>
+    <tableColumn id="2" name="this_hue"/>
+    <tableColumn id="4" name="this_inc"/>
+    <tableColumn id="3" name="this_delay"/>
+    <tableColumn id="5" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1997,14 +1994,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B4:Q97"/>
+  <dimension ref="B4:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P81" sqref="P81"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,7 +2022,7 @@
     <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -2057,10 +2054,10 @@
         <v>57</v>
       </c>
       <c r="O4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>65</v>
       </c>
@@ -2092,10 +2089,10 @@
         <v>103</v>
       </c>
       <c r="O5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>66</v>
       </c>
@@ -2128,10 +2125,10 @@
         <v>103</v>
       </c>
       <c r="O6" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>67</v>
       </c>
@@ -2164,10 +2161,10 @@
         <v>103</v>
       </c>
       <c r="O7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>68</v>
       </c>
@@ -2200,10 +2197,10 @@
         <v>104</v>
       </c>
       <c r="O8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>69</v>
       </c>
@@ -2231,8 +2228,11 @@
       <c r="M9" s="18" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>70</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>71</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>72</v>
       </c>
@@ -2331,16 +2331,19 @@
         <v>108</v>
       </c>
       <c r="O12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="P12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="Q12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="R12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>73</v>
       </c>
@@ -2376,13 +2379,13 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="Q13" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>74</v>
       </c>
@@ -2418,13 +2421,13 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="Q14" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>75</v>
       </c>
@@ -2460,13 +2463,13 @@
         <v>2</v>
       </c>
       <c r="P15" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="Q15" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>76</v>
       </c>
@@ -2502,13 +2505,13 @@
         <v>3</v>
       </c>
       <c r="P16" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="Q16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>77</v>
       </c>
@@ -2537,8 +2540,20 @@
       <c r="M17" s="18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>4</v>
+      </c>
+      <c r="P17" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>249</v>
+      </c>
+      <c r="R17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>78</v>
       </c>
@@ -2571,7 +2586,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>79</v>
       </c>
@@ -2604,7 +2619,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>80</v>
       </c>
@@ -2634,7 +2649,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>81</v>
       </c>
@@ -2667,7 +2682,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>82</v>
       </c>
@@ -2700,7 +2715,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>83</v>
       </c>
@@ -2733,7 +2748,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>84</v>
       </c>
@@ -2766,7 +2781,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>85</v>
       </c>
@@ -2780,7 +2795,7 @@
         <v>46</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J25" s="8"/>
       <c r="L25">
@@ -2791,7 +2806,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>86</v>
       </c>
@@ -2818,7 +2833,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>87</v>
       </c>
@@ -2843,7 +2858,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>88</v>
       </c>
@@ -2870,7 +2885,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>89</v>
       </c>
@@ -2884,7 +2899,7 @@
         <v>53</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>54</v>
@@ -2897,7 +2912,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>90</v>
       </c>
@@ -2911,7 +2926,7 @@
         <v>55</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>54</v>
@@ -2924,7 +2939,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="L31">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2933,7 +2948,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="L32">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3182,7 +3197,7 @@
         <v>54</v>
       </c>
       <c r="M59" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="12:13" x14ac:dyDescent="0.25">
@@ -3191,7 +3206,7 @@
         <v>55</v>
       </c>
       <c r="M60" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="12:13" x14ac:dyDescent="0.25">
@@ -3209,7 +3224,7 @@
         <v>57</v>
       </c>
       <c r="M62" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="12:13" x14ac:dyDescent="0.25">
@@ -3218,7 +3233,7 @@
         <v>58</v>
       </c>
       <c r="M63" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="12:13" x14ac:dyDescent="0.25">
@@ -3236,7 +3251,7 @@
         <v>60</v>
       </c>
       <c r="M65" s="18" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="12:13" x14ac:dyDescent="0.25">
@@ -3245,7 +3260,7 @@
         <v>61</v>
       </c>
       <c r="M66" s="18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="12:13" x14ac:dyDescent="0.25">
@@ -3539,11 +3554,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="77" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView topLeftCell="A22" zoomScale="77" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,7 +3601,7 @@
         <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I3" t="s">
         <v>40</v>
@@ -4121,7 +4136,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
@@ -4155,11 +4170,11 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K22" s="1">
         <v>1</v>
@@ -4237,7 +4252,7 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
@@ -4271,11 +4286,11 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K27" s="1">
         <v>1</v>
@@ -4305,11 +4320,11 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K28" s="1">
         <v>128</v>
@@ -4339,11 +4354,11 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K29" s="1">
         <v>80</v>
@@ -4387,7 +4402,7 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
@@ -4425,20 +4440,20 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K32" s="1">
         <v>1</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="N32" s="1"/>
     </row>
@@ -4463,20 +4478,20 @@
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K33" s="1">
         <v>32</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N33" s="1"/>
     </row>
@@ -4501,20 +4516,20 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K34" s="1">
         <v>128</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N34" s="1"/>
     </row>
@@ -4539,20 +4554,20 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K35" s="1">
         <v>80</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N35" s="1"/>
     </row>
@@ -4577,20 +4592,20 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K36" s="1">
         <v>1</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N36" s="1"/>
     </row>
@@ -4615,11 +4630,11 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="K37" s="1">
         <v>1</v>
@@ -4628,7 +4643,7 @@
         <v>108115103109</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N37" s="1"/>
     </row>
@@ -4650,7 +4665,7 @@
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1" t="s">
@@ -4688,20 +4703,20 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K39" s="1">
         <v>48</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N39" s="1"/>
     </row>
@@ -4748,7 +4763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K18"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
@@ -4786,10 +4801,10 @@
         <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -4843,7 +4858,7 @@
         <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -4979,7 +4994,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
@@ -5054,7 +5069,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5088,31 +5103,31 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" t="s">
         <v>175</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>176</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>177</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>178</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>179</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>180</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>181</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>182</v>
-      </c>
-      <c r="M5" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -5152,7 +5167,7 @@
         <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -5168,7 +5183,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -5230,7 +5245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I20"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -5261,13 +5276,13 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5466,7 +5481,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -5545,7 +5560,7 @@
         <v>27</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -5570,7 +5585,7 @@
         <v>22</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -5609,7 +5624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:L14"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -5863,7 +5878,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5930,7 +5945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -6091,7 +6106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6189,7 +6204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F14"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -6319,7 +6334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:O22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -6820,11 +6835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6857,7 +6872,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6887,8 +6902,8 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>184</v>
+      <c r="E5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6904,8 +6919,8 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>171</v>
+      <c r="E6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -6921,8 +6936,8 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
-        <v>185</v>
+      <c r="E7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -6956,7 +6971,7 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -7002,7 +7017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7072,7 +7087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -7309,7 +7324,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:N19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -7367,7 +7382,7 @@
         <v>15</v>
       </c>
       <c r="N4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -7836,10 +7851,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -8081,7 +8096,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8164,7 +8179,7 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -8186,7 +8201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8210,7 +8225,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -8224,7 +8239,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -8254,7 +8269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8402,7 +8417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8431,7 +8446,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
@@ -8451,7 +8466,7 @@
         <v>165</v>
       </c>
       <c r="G6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
@@ -8476,7 +8491,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
@@ -8503,7 +8518,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I38"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
@@ -8546,7 +8561,7 @@
         <v>116</v>
       </c>
       <c r="I3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -8875,10 +8890,10 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I22" s="1"/>
     </row>
@@ -8942,10 +8957,10 @@
         <v>97</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I26" s="1"/>
     </row>
@@ -8968,7 +8983,7 @@
         <v>101100115110</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I27" s="1"/>
     </row>
@@ -8988,10 +9003,10 @@
         <v>74</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I28" s="1"/>
     </row>
@@ -9011,10 +9026,10 @@
         <v>51</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -9050,10 +9065,10 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I31" s="1"/>
     </row>
@@ -9074,7 +9089,7 @@
         <v>120110115130</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I32" s="1"/>
     </row>
@@ -9126,10 +9141,10 @@
         <v>68</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I35" s="1"/>
     </row>
@@ -9149,10 +9164,10 @@
         <v>51</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -9172,10 +9187,10 @@
         <v>73</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -9206,7 +9221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9233,13 +9248,13 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -9264,19 +9279,19 @@
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -9285,7 +9300,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -9294,7 +9309,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>

</xml_diff>